<commit_message>
VAN-1811:Prepare and write  FUNCTIONAL test cases and test scripts
</commit_message>
<xml_diff>
--- a/ui-testsuite/src/main/resources/TestData/ATR_Imported_ByNegativeOrder.xlsx
+++ b/ui-testsuite/src/main/resources/TestData/ATR_Imported_ByNegativeOrder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Pipeline\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Workspace\ui-test\ui-testsuite\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$FF$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -1114,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FF2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BL1" workbookViewId="0">
-      <selection activeCell="BT3" sqref="BT3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>